<commit_message>
rebalance data option added
</commit_message>
<xml_diff>
--- a/results/scores_agr_a.xlsx
+++ b/results/scores_agr_a.xlsx
@@ -408,13 +408,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.9075</v>
+        <v>0.9184</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9192</v>
+        <v>0.9307</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9064</v>
+        <v>0.9076</v>
       </c>
     </row>
     <row r="3">
@@ -432,13 +432,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.8283</v>
+        <v>0.9152</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9036999999999999</v>
+        <v>0.9256</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8907</v>
+        <v>0.911</v>
       </c>
     </row>
     <row r="4">
@@ -456,13 +456,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.1174</v>
+        <v>0.0058</v>
       </c>
       <c r="E4" t="n">
-        <v>0.032</v>
+        <v>0.008699999999999999</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0419</v>
+        <v>0.0073</v>
       </c>
     </row>
     <row r="5">
@@ -480,13 +480,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.9421</v>
+        <v>0.9488</v>
       </c>
       <c r="E5" t="n">
-        <v>0.944</v>
+        <v>0.953</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9385</v>
+        <v>0.9392</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.8159999999999999</v>
+        <v>0.9471000000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9076</v>
+        <v>0.9504</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8966</v>
+        <v>0.9408</v>
       </c>
     </row>
     <row r="7">
@@ -528,13 +528,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.1625</v>
+        <v>0.0033</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0552</v>
+        <v>0.0051</v>
       </c>
       <c r="F7" t="n">
-        <v>0.065</v>
+        <v>0.0039</v>
       </c>
     </row>
     <row r="8">
@@ -552,13 +552,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>32.0455</v>
+        <v>10.9161</v>
       </c>
       <c r="E8" t="n">
-        <v>47.698</v>
+        <v>7.842</v>
       </c>
       <c r="F8" t="n">
-        <v>199.7032</v>
+        <v>25.4019</v>
       </c>
     </row>
     <row r="9">
@@ -576,13 +576,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>3.259</v>
+        <v>5.0981</v>
       </c>
       <c r="E9" t="n">
-        <v>5.9014</v>
+        <v>0.8905999999999999</v>
       </c>
       <c r="F9" t="n">
-        <v>6.8536</v>
+        <v>0.8068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>